<commit_message>
Picture upload and image
</commit_message>
<xml_diff>
--- a/Data/Vechile Inspection.xlsx
+++ b/Data/Vechile Inspection.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Store</t>
   </si>
@@ -74,6 +73,72 @@
   </si>
   <si>
     <t>14785236901478529</t>
+  </si>
+  <si>
+    <t>GPSID</t>
+  </si>
+  <si>
+    <t>145698723078</t>
+  </si>
+  <si>
+    <t>Driver Side Image</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\DriverSide.png</t>
+  </si>
+  <si>
+    <t>Passanger Side Image</t>
+  </si>
+  <si>
+    <t>Fornt Image</t>
+  </si>
+  <si>
+    <t>Rear Image</t>
+  </si>
+  <si>
+    <t>VIN Image</t>
+  </si>
+  <si>
+    <t>Engine Bay Image</t>
+  </si>
+  <si>
+    <t>Interior Image</t>
+  </si>
+  <si>
+    <t>Odometer Image</t>
+  </si>
+  <si>
+    <t>GPS Installation</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\PassengerSide.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\FrontSide.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\RearSide.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\VIN.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\Engine_Bay.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\Interior_DriverSide.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\Odometer.png</t>
+  </si>
+  <si>
+    <t>GPSID Number Image</t>
+  </si>
+  <si>
+    <t>C:\\Users\\barga\\git\\AutoTitleLoanApp\\Images\\GPS_ID.png</t>
+  </si>
+  <si>
+    <t>Visakhapatnam</t>
   </si>
 </sst>
 </file>
@@ -115,10 +180,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,19 +489,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1"/>
+    <col min="18" max="18" width="18" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.42578125" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +549,41 @@
       <c r="L1" t="s">
         <v>14</v>
       </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -506,10 +619,44 @@
       </c>
       <c r="L2" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>